<commit_message>
include exclusion line (at least one outcome)
</commit_message>
<xml_diff>
--- a/sensitivity-analysis/tables/log-odds/binaryattitude3.xlsx
+++ b/sensitivity-analysis/tables/log-odds/binaryattitude3.xlsx
@@ -29732,13 +29732,13 @@
         <v>-0.43142696079097809</v>
       </c>
       <c r="C3" s="622">
-        <v>0.38690423014398778</v>
+        <v>0.38690423014398795</v>
       </c>
       <c r="D3" s="626">
-        <v>-1.2068003648435377</v>
+        <v>-1.2068003648435379</v>
       </c>
       <c r="E3" s="630">
-        <v>0.34394644326158152</v>
+        <v>0.34394644326158186</v>
       </c>
     </row>
   </sheetData>
@@ -29852,13 +29852,13 @@
         <v>0.54174285929342569</v>
       </c>
       <c r="C3" s="730">
-        <v>0.35426776511328345</v>
+        <v>0.35426776511328334</v>
       </c>
       <c r="D3" s="734">
-        <v>-0.16822560726935243</v>
+        <v>-0.16822560726935221</v>
       </c>
       <c r="E3" s="738">
-        <v>1.2517113258562038</v>
+        <v>1.2517113258562036</v>
       </c>
     </row>
   </sheetData>
@@ -30169,13 +30169,13 @@
         <v>-0.82344291924040136</v>
       </c>
       <c r="C4" s="1015">
-        <v>0.49700684579381071</v>
+        <v>0.49700684579381077</v>
       </c>
       <c r="D4" s="1019">
-        <v>-1.8194668958124778</v>
+        <v>-1.819466895812478</v>
       </c>
       <c r="E4" s="1023">
-        <v>0.17258105733167517</v>
+        <v>0.17258105733167528</v>
       </c>
     </row>
   </sheetData>
@@ -30777,10 +30777,10 @@
         <v>0.77778725234279589</v>
       </c>
       <c r="C3" s="1504">
-        <v>0.47936107147881285</v>
+        <v>0.47936107147881291</v>
       </c>
       <c r="D3" s="1507">
-        <v>-0.18287380226621164</v>
+        <v>-0.18287380226621175</v>
       </c>
       <c r="E3" s="1510">
         <v>1.7384483069518035</v>
@@ -30974,10 +30974,10 @@
         <v>0.37115340333860586</v>
       </c>
       <c r="C3" s="1684">
-        <v>0.36521167024508611</v>
+        <v>0.36521167024508605</v>
       </c>
       <c r="D3" s="1688">
-        <v>-0.36074713921237261</v>
+        <v>-0.3607471392123725</v>
       </c>
       <c r="E3" s="1692">
         <v>1.1030539458895843</v>
@@ -31034,13 +31034,13 @@
         <v>0.15213084636255042</v>
       </c>
       <c r="C3" s="1738">
-        <v>0.70951323906430697</v>
+        <v>0.70951323906430686</v>
       </c>
       <c r="D3" s="1742">
-        <v>-1.2697654590588545</v>
+        <v>-1.2697654590588543</v>
       </c>
       <c r="E3" s="1746">
-        <v>1.5740271517839552</v>
+        <v>1.574027151783955</v>
       </c>
     </row>
   </sheetData>
@@ -31445,13 +31445,13 @@
         <v>0.1720484163915646</v>
       </c>
       <c r="C3" s="322">
-        <v>0.39058472151286738</v>
+        <v>0.39058472151286727</v>
       </c>
       <c r="D3" s="326">
-        <v>-0.6107008571887389</v>
+        <v>-0.61070085718873868</v>
       </c>
       <c r="E3" s="330">
-        <v>0.95479768997186798</v>
+        <v>0.95479768997186776</v>
       </c>
     </row>
   </sheetData>
@@ -31642,10 +31642,10 @@
         <v>1.0575263268733197</v>
       </c>
       <c r="C3" s="499">
-        <v>0.35365371625345471</v>
+        <v>0.35365371625345476</v>
       </c>
       <c r="D3" s="503">
-        <v>0.34878844172476597</v>
+        <v>0.34878844172476586</v>
       </c>
       <c r="E3" s="507">
         <v>1.7662642120218734</v>
@@ -31719,10 +31719,10 @@
         <v>1.7410669948574564</v>
       </c>
       <c r="C4" s="568">
-        <v>0.46956798920113979</v>
+        <v>0.46956798920113985</v>
       </c>
       <c r="D4" s="572">
-        <v>0.80003171569934095</v>
+        <v>0.80003171569934084</v>
       </c>
       <c r="E4" s="576">
         <v>2.682102274015572</v>

</xml_diff>